<commit_message>
Updated Bell ring mode
</commit_message>
<xml_diff>
--- a/question/question.xlsx
+++ b/question/question.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aslam\Desktop\math v2\Maths-Tutor-QT-V2\question\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIDDHANT\Desktop\Zendalona\forkedFolder\Maths-Tutor-QT-V2\question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B60452-271C-4C65-8042-07D1F1815677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736578FE-E4AD-4271-84E1-D2EF3016C4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="115">
   <si>
     <t>question</t>
   </si>
@@ -234,18 +229,9 @@
     <t>Remainder</t>
   </si>
   <si>
-    <t>Ramu has {x} apples</t>
-  </si>
-  <si>
     <t>Bellring</t>
   </si>
   <si>
-    <t>x1:5</t>
-  </si>
-  <si>
-    <t>{x}</t>
-  </si>
-  <si>
     <t>{a} + {b} + {c} =</t>
   </si>
   <si>
@@ -298,19 +284,107 @@
   </si>
   <si>
     <t>questin_hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} + {b} = </t>
+  </si>
+  <si>
+    <t>a1:9*b1:9*</t>
+  </si>
+  <si>
+    <t>a2:5*b2:5*</t>
+  </si>
+  <si>
+    <t>a2;1;4*b2;1;1*</t>
+  </si>
+  <si>
+    <t>a2;1;4*b1:5*</t>
+  </si>
+  <si>
+    <t>a3;1;3*b1:3*</t>
+  </si>
+  <si>
+    <t>{a} + {b} =</t>
+  </si>
+  <si>
+    <t>a5;1;1*b1:9*</t>
+  </si>
+  <si>
+    <t>a1:5*b1:5*</t>
+  </si>
+  <si>
+    <t>a1:9*b1:1*</t>
+  </si>
+  <si>
+    <t>a1:7*b2:2*</t>
+  </si>
+  <si>
+    <t>a2;1;4*b2;1;4*</t>
+  </si>
+  <si>
+    <t>a3:3*b1:6*</t>
+  </si>
+  <si>
+    <t>a3:7*b1:2*</t>
+  </si>
+  <si>
+    <t>a2:9*b1:1*</t>
+  </si>
+  <si>
+    <t>a6:9*b1:5*</t>
+  </si>
+  <si>
+    <t>a3:9*b2:2*</t>
+  </si>
+  <si>
+    <t>a9:9*b1:8*</t>
+  </si>
+  <si>
+    <t>a2:2*b1:4*</t>
+  </si>
+  <si>
+    <t>a3:3*b1:3*</t>
+  </si>
+  <si>
+    <t>a1:3*b1:3*</t>
+  </si>
+  <si>
+    <t>a4:4*b1:2*</t>
+  </si>
+  <si>
+    <t>a5:5*b1:1*</t>
+  </si>
+  <si>
+    <t>a2;1;4*b2:2*</t>
+  </si>
+  <si>
+    <t>a3;1;3*b3:3*</t>
+  </si>
+  <si>
+    <t>a4;1;2*b4:4*</t>
+  </si>
+  <si>
+    <t>a6:6*b1,2,3,6*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -337,18 +411,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{B1D62F87-E836-49DE-B376-913AFF07DE99}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,9 +441,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -404,7 +481,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -510,7 +587,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -652,7 +729,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -660,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -718,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -741,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -764,7 +841,7 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -787,7 +864,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -810,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -833,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -856,7 +933,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -879,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -902,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -925,7 +1002,7 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -948,7 +1025,7 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -971,7 +1048,7 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -994,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1017,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1040,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1063,7 +1140,7 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1086,7 +1163,7 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1109,7 +1186,7 @@
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1132,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1155,7 +1232,7 @@
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1178,7 +1255,7 @@
         <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1201,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1224,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1270,30 +1347,651 @@
         <v>10</v>
       </c>
       <c r="G26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="3">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="3">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="3">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="3">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="3">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="3">
+        <v>10</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="3">
+        <v>10</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="3">
+        <v>10</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="3">
+        <v>10</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="3">
+        <v>10</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="3">
+        <v>10</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="3">
+        <v>10</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F27">
-        <v>10</v>
-      </c>
-      <c r="G27" t="s">
-        <v>89</v>
+      <c r="B39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="3">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="3">
+        <v>10</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="3">
+        <v>10</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="3">
+        <v>10</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="3">
+        <v>10</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="3">
+        <v>10</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="3">
+        <v>10</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="3">
+        <v>10</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="3">
+        <v>10</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="3">
+        <v>10</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="3">
+        <v>10</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="3">
+        <v>10</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" s="3">
+        <v>10</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" s="3">
+        <v>10</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="3">
+        <v>10</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" s="3">
+        <v>10</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>